<commit_message>
Nuevo arreglo en formulas
</commit_message>
<xml_diff>
--- a/preguntas_relacionadas/p_formula.xlsx
+++ b/preguntas_relacionadas/p_formula.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://365inegi-my.sharepoint.com/personal/aaron_ramirez_inegi_org_mx/Documents/Documents/codigos_python/Prueba2_p_rel/P_rel_git/preguntas_relacionadas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{C3F943BD-552F-4F45-9F90-B595D957DDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EC2A590-5074-4208-8261-DCEDC6212D3E}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{C3F943BD-552F-4F45-9F90-B595D957DDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{830E8D80-2C32-4107-B206-80644642BD68}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A595293E-8E41-4F55-AF5A-447CE0A3C184}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>A1</t>
   </si>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>A3.1&lt;</t>
-  </si>
-  <si>
-    <t>a4+</t>
-  </si>
-  <si>
-    <t>a4.1=</t>
   </si>
   <si>
     <t>a5:</t>
@@ -450,7 +444,7 @@
   <dimension ref="Z4:AE12"/>
   <sheetViews>
     <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5:Z9"/>
+      <selection activeCell="AC5" sqref="AC5:AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,22 +456,16 @@
     </row>
     <row r="5" spans="26:31" x14ac:dyDescent="0.25">
       <c r="Z5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AB5" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="26:31" x14ac:dyDescent="0.25">
       <c r="AB6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AC6" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="7" spans="26:31" x14ac:dyDescent="0.25">
       <c r="AA7" s="1" t="s">
@@ -492,7 +480,7 @@
     </row>
     <row r="9" spans="26:31" x14ac:dyDescent="0.25">
       <c r="Z9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="26:31" x14ac:dyDescent="0.25">
@@ -523,27 +511,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71C443C-FF75-4A25-8507-182EEF19AED5}">
-  <dimension ref="D9:G15"/>
+  <dimension ref="AC14:AE21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="X7" workbookViewId="0">
+      <selection activeCell="AI20" sqref="AI20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+    <row r="14" spans="31:31" x14ac:dyDescent="0.25">
+      <c r="AE14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="29:29" x14ac:dyDescent="0.25">
+      <c r="AC17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="G15" t="s">
-        <v>12</v>
+    <row r="21" spans="29:29" x14ac:dyDescent="0.25">
+      <c r="AC21" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>